<commit_message>
tweaks for updated Hyperdrive functionality
</commit_message>
<xml_diff>
--- a/HealthcareSolutions.suite/Resources/HDREG-1.xlsx
+++ b/HealthcareSolutions.suite/Resources/HDREG-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScriptRepositories\Eggplant\WVUMed.suite\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScriptRepositories\HealthcareSolutions\HealthcareSolutions.suite\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FC715F-8483-45FE-A82A-B648A1416174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C05B47-85CF-4047-A36E-17C703BF057C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120"/>
   </bookViews>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="422">
   <si>
     <t>RecNumber</t>
   </si>
@@ -1522,33 +1522,15 @@
     <t>11011999</t>
   </si>
   <si>
-    <t>E33009052</t>
-  </si>
-  <si>
-    <t>E33008994</t>
-  </si>
-  <si>
-    <t>E33008993</t>
-  </si>
-  <si>
     <t>11011990</t>
   </si>
   <si>
-    <t>E33008978</t>
-  </si>
-  <si>
     <t>100096</t>
   </si>
   <si>
     <t>11012009</t>
   </si>
   <si>
-    <t>E33009272</t>
-  </si>
-  <si>
-    <t>E33009299</t>
-  </si>
-  <si>
     <t>InsuranceID_Type</t>
   </si>
   <si>
@@ -1558,31 +1540,13 @@
     <t>Recipient Number</t>
   </si>
   <si>
-    <t>E33009300</t>
-  </si>
-  <si>
     <t>United Healthcare</t>
   </si>
   <si>
-    <t>E33009301</t>
-  </si>
-  <si>
-    <t>E33009302</t>
-  </si>
-  <si>
-    <t>E33009303</t>
-  </si>
-  <si>
-    <t>E33009304</t>
-  </si>
-  <si>
-    <t>E33009305</t>
-  </si>
-  <si>
     <t>Blue Cross</t>
   </si>
   <si>
-    <t>E33009306</t>
+    <t>361636</t>
   </si>
 </sst>
 </file>
@@ -2076,7 +2040,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS1" sqref="AS1:AS1048576"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2272,7 +2236,7 @@
         <v>16</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="AV1" s="2" t="s">
         <v>24</v>
@@ -2295,7 +2259,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C2" s="3" t="str">
         <f t="shared" ref="C2:C32" si="0">CONCATENATE(E2,", ",D2)</f>
@@ -2420,7 +2384,7 @@
         <v>294</v>
       </c>
       <c r="AS2" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT2" s="3">
         <v>1652</v>
@@ -2437,13 +2401,13 @@
       <c r="AY2" s="3" t="s">
         <v>408</v>
       </c>
+      <c r="AZ2" s="5" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="3" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>415</v>
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" si="0"/>
@@ -2456,7 +2420,7 @@
         <v>88</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
@@ -2596,9 +2560,6 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>414</v>
-      </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Jackson</v>
@@ -2610,7 +2571,7 @@
         <v>88</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
@@ -2722,7 +2683,7 @@
         <v>294</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT4" s="3">
         <v>1402</v>
@@ -2744,9 +2705,6 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>413</v>
-      </c>
       <c r="C5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Emma</v>
@@ -2758,7 +2716,7 @@
         <v>88</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
@@ -2876,7 +2834,7 @@
         <v>360</v>
       </c>
       <c r="AS5" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT5" s="3">
         <v>1652</v>
@@ -2984,7 +2942,7 @@
         <v>354</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AH6" s="3" t="s">
         <v>38</v>
@@ -3039,9 +2997,6 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>420</v>
-      </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Olivia</v>
@@ -3053,7 +3008,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>25</v>
@@ -3161,7 +3116,7 @@
         <v>360</v>
       </c>
       <c r="AS7" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT7" s="3">
         <v>1402</v>
@@ -3194,7 +3149,7 @@
         <v>88</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>17</v>
@@ -3302,13 +3257,13 @@
         <v>294</v>
       </c>
       <c r="AS8" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT8" s="3">
         <v>1652</v>
       </c>
       <c r="AU8" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="AV8" s="3" t="s">
         <v>410</v>
@@ -3330,9 +3285,6 @@
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>421</v>
-      </c>
       <c r="C9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Isabella</v>
@@ -3344,7 +3296,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>25</v>
@@ -3458,7 +3410,7 @@
         <v>1546</v>
       </c>
       <c r="AU9" s="3" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="AV9" s="3">
         <v>98523601207</v>
@@ -3480,9 +3432,6 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>425</v>
-      </c>
       <c r="C10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Mason</v>
@@ -3494,7 +3443,7 @@
         <v>88</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>17</v>
@@ -3602,13 +3551,13 @@
         <v>294</v>
       </c>
       <c r="AS10" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT10" s="3">
         <v>1402</v>
       </c>
       <c r="AU10" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="AV10" s="3" t="s">
         <v>367</v>
@@ -3630,9 +3579,6 @@
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>427</v>
-      </c>
       <c r="C11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Ava</v>
@@ -3644,7 +3590,7 @@
         <v>88</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>25</v>
@@ -3752,13 +3698,13 @@
         <v>360</v>
       </c>
       <c r="AS11" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT11" s="3">
         <v>1652</v>
       </c>
       <c r="AU11" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="AV11" s="3" t="s">
         <v>410</v>
@@ -3780,9 +3726,7 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>428</v>
-      </c>
+      <c r="B12" s="7"/>
       <c r="C12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Noah</v>
@@ -3794,7 +3738,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>17</v>
@@ -3908,7 +3852,7 @@
         <v>1546</v>
       </c>
       <c r="AU12" s="3" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="AV12" s="3">
         <v>98523601207</v>
@@ -3930,9 +3874,6 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>429</v>
-      </c>
       <c r="C13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Lily</v>
@@ -3944,7 +3885,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>25</v>
@@ -4052,13 +3993,13 @@
         <v>360</v>
       </c>
       <c r="AS13" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT13" s="3">
         <v>1402</v>
       </c>
       <c r="AU13" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="AV13" s="3" t="s">
         <v>367</v>
@@ -4080,9 +4021,7 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>430</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Michael</v>
@@ -4094,7 +4033,7 @@
         <v>88</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>17</v>
@@ -4202,13 +4141,13 @@
         <v>294</v>
       </c>
       <c r="AS14" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT14" s="3">
         <v>1652</v>
       </c>
       <c r="AU14" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="AV14" s="3" t="s">
         <v>410</v>
@@ -4230,9 +4169,6 @@
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>431</v>
-      </c>
       <c r="C15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Jessica</v>
@@ -4356,13 +4292,13 @@
         <v>294</v>
       </c>
       <c r="AS15" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT15" s="3">
         <v>1652</v>
       </c>
       <c r="AU15" s="3" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="AV15" s="3" t="s">
         <v>410</v>
@@ -4384,9 +4320,6 @@
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>433</v>
-      </c>
       <c r="C16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>Eggplant, Christopher</v>
@@ -4522,7 +4455,7 @@
         <v>1546</v>
       </c>
       <c r="AU16" s="3" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="AV16" s="3">
         <v>98523601207</v>
@@ -4667,7 +4600,7 @@
         <v>294</v>
       </c>
       <c r="AS17" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT17" s="3">
         <v>1402</v>
@@ -4818,7 +4751,7 @@
         <v>360</v>
       </c>
       <c r="AS18" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT18" s="3">
         <v>1652</v>
@@ -5114,7 +5047,7 @@
         <v>360</v>
       </c>
       <c r="AS20" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT20" s="3">
         <v>1402</v>
@@ -5259,7 +5192,7 @@
         <v>294</v>
       </c>
       <c r="AS21" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT21" s="3">
         <v>1652</v>
@@ -5555,7 +5488,7 @@
         <v>294</v>
       </c>
       <c r="AS23" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT23" s="3">
         <v>1402</v>
@@ -5706,7 +5639,7 @@
         <v>360</v>
       </c>
       <c r="AS24" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT24" s="3">
         <v>1652</v>
@@ -6002,7 +5935,7 @@
         <v>360</v>
       </c>
       <c r="AS26" s="3" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="AT26" s="3">
         <v>1402</v>
@@ -6105,7 +6038,7 @@
         <v>294</v>
       </c>
       <c r="AS27" s="3" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="AT27" s="3">
         <v>1652</v>
@@ -11077,6 +11010,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E033184CEB11F648BBD0F70F1BE6A53E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6772e668bd11b5d68af2caf9f3d3ff0e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a44a327f-4c77-4059-bb07-e278862d87fb" xmlns:ns4="7fa3c9fb-ef78-47d6-a04f-8ab7fe78f626" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1370a7ae997dfead2b2ac8f1c36ed42" ns3:_="" ns4:_="">
     <xsd:import namespace="a44a327f-4c77-4059-bb07-e278862d87fb"/>
@@ -11299,36 +11247,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4BE07B4-EAD3-43BB-A412-78B98636CC41}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA715A9A-50E5-49B3-81AC-118F4B5A14E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a44a327f-4c77-4059-bb07-e278862d87fb"/>
-    <ds:schemaRef ds:uri="7fa3c9fb-ef78-47d6-a04f-8ab7fe78f626"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11351,9 +11273,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA715A9A-50E5-49B3-81AC-118F4B5A14E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4BE07B4-EAD3-43BB-A412-78B98636CC41}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a44a327f-4c77-4059-bb07-e278862d87fb"/>
+    <ds:schemaRef ds:uri="7fa3c9fb-ef78-47d6-a04f-8ab7fe78f626"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>